<commit_message>
amended temaplate - kpi fixed
</commit_message>
<xml_diff>
--- a/Projects/SANOFIZA/Data/Template.xlsx
+++ b/Projects/SANOFIZA/Data/Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="MSL" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Primary Shelf_Location" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Primary Shelf_Location" sheetId="3" state="hidden" r:id="rId4"/>
     <sheet name="Primary_Brand_Blocking" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Primary&amp;Secondary_POSM" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="Primary&amp;Secondary_Facings" sheetId="6" state="visible" r:id="rId7"/>
@@ -297,7 +297,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="132">
   <si>
     <t xml:space="preserve">KPI Name</t>
   </si>
@@ -578,6 +578,12 @@
     <t xml:space="preserve">Shelf Location Compliance</t>
   </si>
   <si>
+    <t xml:space="preserve">Enterogermina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENTEROGERMINA SUSP 5ML 10 BOT</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mega</t>
   </si>
   <si>
@@ -683,7 +689,7 @@
     <t xml:space="preserve">Mega Pharmacies</t>
   </si>
   <si>
-    <t xml:space="preserve">Product Minimum Facing Secondary </t>
+    <t xml:space="preserve">Product Minimum Facings Secondary </t>
   </si>
   <si>
     <t xml:space="preserve">S-CT-03</t>
@@ -1065,7 +1071,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="97">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1206,6 +1212,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="18" fillId="6" borderId="5" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1292,6 +1302,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="9" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1436,6 +1450,14 @@
     </xf>
     <xf numFmtId="164" fontId="21" fillId="12" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1518,19 +1540,19 @@
   </sheetPr>
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.0647773279352"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.2793522267206"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.8542510121457"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.8542510121457"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.0647773279352"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.1052631578947"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.7449392712551"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.5303643724696"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1773,10 +1795,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="21" width="25.0647773279352"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="21" width="43.0607287449393"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="21" width="22.0647773279352"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="21" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="21" width="24.8502024291498"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="21" width="42.6315789473684"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="21" width="21.8542510121457"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="21" width="17.7813765182186"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="21" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="7" min="6" style="21" width="9.4251012145749"/>
     <col collapsed="false" hidden="false" max="9" min="8" style="22" width="9.4251012145749"/>
@@ -2587,215 +2609,227 @@
   </sheetPr>
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="34" width="25.0647773279352"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="34" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="34" width="31.0647773279352"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="34" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="34" width="17.246963562753"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="22" width="8.89068825910931"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="34" width="24.8502024291498"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="34" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="34" width="30.7449392712551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="34" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="34" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="35" width="8.89068825910931"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="35"/>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
+    <row r="1" s="22" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="36"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
       <c r="F1" s="24" t="s">
         <v>27</v>
       </c>
       <c r="G1" s="24"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="36" t="s">
+      <c r="A2" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="36" t="s">
+      <c r="D2" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="E2" s="36" t="s">
+      <c r="E2" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="37" t="s">
+      <c r="F2" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="G2" s="38" t="s">
+      <c r="G2" s="39" t="s">
         <v>91</v>
       </c>
-      <c r="H2" s="39"/>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="40" t="s">
+      <c r="H2" s="40"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="41" t="s">
         <v>92</v>
       </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="40" t="s">
+      <c r="B3" s="42" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="43" t="s">
+        <v>94</v>
+      </c>
+      <c r="E3" s="21" t="n">
+        <v>311922</v>
+      </c>
+      <c r="F3" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="44" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="41" t="s">
         <v>92</v>
       </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="45"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="40" t="s">
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="46"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="41" t="s">
         <v>92</v>
       </c>
-      <c r="B5" s="44"/>
-      <c r="C5" s="44"/>
-      <c r="D5" s="45"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="43"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="46"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="41" t="s">
         <v>92</v>
       </c>
-      <c r="B6" s="44"/>
-      <c r="C6" s="44"/>
-      <c r="D6" s="45"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
+      <c r="B6" s="45"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="46"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="40" t="s">
+      <c r="A7" s="41" t="s">
         <v>92</v>
       </c>
-      <c r="B7" s="44"/>
-      <c r="C7" s="44"/>
-      <c r="D7" s="45"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
+      <c r="B7" s="45"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="46"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="44"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="41" t="s">
         <v>92</v>
       </c>
-      <c r="B8" s="44"/>
-      <c r="C8" s="44"/>
-      <c r="D8" s="45"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="46"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="40" t="s">
+      <c r="A9" s="41" t="s">
         <v>92</v>
       </c>
-      <c r="B9" s="44"/>
-      <c r="C9" s="44"/>
-      <c r="D9" s="45"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
+      <c r="B9" s="45"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="46"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="40" t="s">
+      <c r="A10" s="41" t="s">
         <v>92</v>
       </c>
-      <c r="B10" s="44"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="45"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
+      <c r="B10" s="45"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="46"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="40" t="s">
+      <c r="A11" s="41" t="s">
         <v>92</v>
       </c>
-      <c r="B11" s="44"/>
-      <c r="C11" s="44"/>
-      <c r="D11" s="45"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
+      <c r="B11" s="45"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="46"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="40" t="s">
+      <c r="A12" s="41" t="s">
         <v>92</v>
       </c>
-      <c r="B12" s="44"/>
-      <c r="C12" s="44"/>
-      <c r="D12" s="45"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
+      <c r="B12" s="45"/>
+      <c r="C12" s="45"/>
+      <c r="D12" s="46"/>
+      <c r="F12" s="44"/>
+      <c r="G12" s="44"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="40" t="s">
+      <c r="A13" s="41" t="s">
         <v>92</v>
       </c>
-      <c r="B13" s="44"/>
-      <c r="C13" s="44"/>
-      <c r="D13" s="45"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
+      <c r="B13" s="45"/>
+      <c r="C13" s="45"/>
+      <c r="D13" s="46"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="44"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="40" t="s">
+      <c r="A14" s="41" t="s">
         <v>92</v>
       </c>
-      <c r="B14" s="44"/>
-      <c r="C14" s="44"/>
-      <c r="D14" s="44"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
+      <c r="B14" s="45"/>
+      <c r="C14" s="45"/>
+      <c r="D14" s="45"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="44"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="40" t="s">
+      <c r="A15" s="41" t="s">
         <v>92</v>
       </c>
-      <c r="B15" s="44"/>
-      <c r="C15" s="44"/>
-      <c r="D15" s="44"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="43"/>
+      <c r="B15" s="45"/>
+      <c r="C15" s="45"/>
+      <c r="D15" s="45"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="41" t="s">
         <v>92</v>
       </c>
-      <c r="B16" s="44"/>
-      <c r="C16" s="44"/>
-      <c r="D16" s="45"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="43"/>
+      <c r="B16" s="45"/>
+      <c r="C16" s="45"/>
+      <c r="D16" s="46"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="44"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="40" t="s">
+      <c r="A17" s="41" t="s">
         <v>92</v>
       </c>
-      <c r="B17" s="44"/>
-      <c r="C17" s="44"/>
-      <c r="D17" s="45"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="43"/>
+      <c r="B17" s="45"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="46"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="44"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="40" t="s">
+      <c r="A18" s="41" t="s">
         <v>92</v>
       </c>
-      <c r="B18" s="44"/>
-      <c r="C18" s="44"/>
-      <c r="D18" s="45"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="43"/>
+      <c r="B18" s="45"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="46"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2820,25 +2854,25 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="46" width="20.7813765182186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="46" width="37.2793522267206"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="46" width="20.7813765182186"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="46" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="46" width="14.8906882591093"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="47" width="8.89068825910931"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="47" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="47" width="36.9554655870445"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="47" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="47" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="47" width="14.7813765182186"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="48" width="8.89068825910931"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="48"/>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
+      <c r="A1" s="49"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
       <c r="F1" s="24" t="s">
         <v>27</v>
       </c>
@@ -2849,34 +2883,34 @@
       <c r="K1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="49" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="36" t="s">
+      <c r="A2" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="36" t="s">
+      <c r="D2" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="36" t="s">
+      <c r="E2" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="50" t="s">
+      <c r="F2" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="50" t="s">
-        <v>93</v>
-      </c>
-      <c r="H2" s="50" t="s">
+      <c r="G2" s="51" t="s">
+        <v>95</v>
+      </c>
+      <c r="H2" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="I2" s="50" t="s">
+      <c r="I2" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="J2" s="50" t="s">
+      <c r="J2" s="51" t="s">
         <v>37</v>
       </c>
       <c r="K2" s="28" t="s">
@@ -2884,7 +2918,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="52" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="29" t="s">
@@ -2894,32 +2928,32 @@
         <v>42</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>94</v>
-      </c>
-      <c r="E3" s="52" t="s">
-        <v>95</v>
-      </c>
-      <c r="F3" s="53" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" s="53" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" s="53" t="n">
-        <v>1</v>
-      </c>
-      <c r="I3" s="53" t="n">
-        <v>1</v>
-      </c>
-      <c r="J3" s="53" t="n">
-        <v>1</v>
-      </c>
-      <c r="K3" s="54" t="n">
+        <v>96</v>
+      </c>
+      <c r="E3" s="53" t="s">
+        <v>97</v>
+      </c>
+      <c r="F3" s="54" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="54" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="54" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" s="54" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" s="54" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" s="55" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="52" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="29" t="s">
@@ -2929,32 +2963,32 @@
         <v>42</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>96</v>
-      </c>
-      <c r="E4" s="52" t="s">
-        <v>97</v>
-      </c>
-      <c r="F4" s="55" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" s="55" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" s="55" t="n">
-        <v>1</v>
-      </c>
-      <c r="I4" s="55" t="n">
-        <v>1</v>
-      </c>
-      <c r="J4" s="55" t="n">
-        <v>1</v>
-      </c>
-      <c r="K4" s="56" t="n">
+        <v>98</v>
+      </c>
+      <c r="E4" s="53" t="s">
+        <v>99</v>
+      </c>
+      <c r="F4" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" s="57" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="51" t="s">
+      <c r="A5" s="52" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="29" t="s">
@@ -2964,32 +2998,32 @@
         <v>61</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>98</v>
-      </c>
-      <c r="E5" s="52" t="s">
-        <v>99</v>
-      </c>
-      <c r="F5" s="55" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" s="55" t="n">
-        <v>1</v>
-      </c>
-      <c r="H5" s="55" t="n">
-        <v>1</v>
-      </c>
-      <c r="I5" s="55" t="n">
-        <v>1</v>
-      </c>
-      <c r="J5" s="55" t="n">
-        <v>1</v>
-      </c>
-      <c r="K5" s="56" t="n">
+        <v>100</v>
+      </c>
+      <c r="E5" s="53" t="s">
+        <v>101</v>
+      </c>
+      <c r="F5" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" s="57" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="51" t="s">
+      <c r="A6" s="52" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="29" t="s">
@@ -2999,32 +3033,32 @@
         <v>61</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E6" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="F6" s="55" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" s="55" t="n">
-        <v>1</v>
-      </c>
-      <c r="H6" s="55" t="n">
-        <v>1</v>
-      </c>
-      <c r="I6" s="55" t="n">
-        <v>1</v>
-      </c>
-      <c r="J6" s="55" t="n">
-        <v>1</v>
-      </c>
-      <c r="K6" s="56" t="n">
+        <v>103</v>
+      </c>
+      <c r="F6" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="K6" s="57" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="51" t="s">
+      <c r="A7" s="52" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="29" t="s">
@@ -3034,32 +3068,32 @@
         <v>74</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>102</v>
-      </c>
-      <c r="E7" s="52" t="s">
-        <v>103</v>
-      </c>
-      <c r="F7" s="55" t="n">
-        <v>1</v>
-      </c>
-      <c r="G7" s="55" t="n">
-        <v>1</v>
-      </c>
-      <c r="H7" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" s="56" t="n">
+        <v>104</v>
+      </c>
+      <c r="E7" s="53" t="s">
+        <v>105</v>
+      </c>
+      <c r="F7" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="57" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="51" t="s">
+      <c r="A8" s="52" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="29" t="s">
@@ -3069,32 +3103,32 @@
         <v>80</v>
       </c>
       <c r="D8" s="29" t="s">
-        <v>104</v>
-      </c>
-      <c r="E8" s="52" t="s">
-        <v>105</v>
-      </c>
-      <c r="F8" s="55" t="n">
-        <v>1</v>
-      </c>
-      <c r="G8" s="55" t="n">
-        <v>1</v>
-      </c>
-      <c r="H8" s="55" t="n">
-        <v>1</v>
-      </c>
-      <c r="I8" s="55" t="n">
-        <v>1</v>
-      </c>
-      <c r="J8" s="55" t="n">
-        <v>1</v>
-      </c>
-      <c r="K8" s="56" t="n">
+        <v>106</v>
+      </c>
+      <c r="E8" s="53" t="s">
+        <v>107</v>
+      </c>
+      <c r="F8" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="K8" s="57" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="51" t="s">
+      <c r="A9" s="52" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="29" t="s">
@@ -3104,27 +3138,27 @@
         <v>86</v>
       </c>
       <c r="D9" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="E9" s="52" t="s">
-        <v>107</v>
-      </c>
-      <c r="F9" s="55" t="n">
-        <v>1</v>
-      </c>
-      <c r="G9" s="55" t="n">
-        <v>1</v>
-      </c>
-      <c r="H9" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" s="55" t="n">
-        <v>1</v>
-      </c>
-      <c r="K9" s="56" t="n">
+        <v>108</v>
+      </c>
+      <c r="E9" s="53" t="s">
+        <v>109</v>
+      </c>
+      <c r="F9" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="K9" s="57" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3157,19 +3191,19 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B33" activeCellId="0" sqref="B33"/>
+      <selection pane="topLeft" activeCell="C35" activeCellId="0" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="34" width="28.4939271255061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="57" width="32.3481781376518"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="34" width="22.0647773279352"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="57" width="26.3522267206478"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="57" width="18.8542510121457"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="34" width="18.5303643724696"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="34" width="17.8906882591093"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="58" width="8.89068825910931"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="58" width="28.2793522267206"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="59" width="32.1376518218623"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="58" width="21.8542510121457"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="59" width="26.1376518218623"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="59" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="58" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="58" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="60" width="8.89068825910931"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3188,34 +3222,34 @@
       <c r="K1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="49" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="36" t="s">
+      <c r="A2" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="36" t="s">
+      <c r="D2" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="36" t="s">
+      <c r="E2" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="50" t="s">
+      <c r="F2" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="50" t="s">
-        <v>93</v>
-      </c>
-      <c r="H2" s="50" t="s">
+      <c r="G2" s="51" t="s">
+        <v>95</v>
+      </c>
+      <c r="H2" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="I2" s="50" t="s">
-        <v>108</v>
-      </c>
-      <c r="J2" s="50" t="s">
+      <c r="I2" s="51" t="s">
+        <v>110</v>
+      </c>
+      <c r="J2" s="51" t="s">
         <v>37</v>
       </c>
       <c r="K2" s="28" t="s">
@@ -3223,328 +3257,328 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="C3" s="61" t="s">
-        <v>110</v>
-      </c>
-      <c r="D3" s="62" t="s">
+      <c r="B3" s="62" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" s="63" t="s">
+        <v>112</v>
+      </c>
+      <c r="D3" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="63" t="s">
+      <c r="E3" s="65" t="s">
         <v>42</v>
       </c>
-      <c r="F3" s="64" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" s="64" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" s="64" t="n">
-        <v>1</v>
-      </c>
-      <c r="I3" s="64" t="n">
-        <v>1</v>
-      </c>
-      <c r="J3" s="64" t="n">
-        <v>1</v>
-      </c>
-      <c r="K3" s="65" t="n">
+      <c r="F3" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" s="67" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="59" t="s">
+      <c r="A4" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="60" t="s">
-        <v>111</v>
-      </c>
-      <c r="C4" s="61" t="s">
-        <v>112</v>
-      </c>
-      <c r="D4" s="62" t="s">
+      <c r="B4" s="62" t="s">
         <v>113</v>
       </c>
-      <c r="E4" s="63" t="s">
+      <c r="C4" s="63" t="s">
         <v>114</v>
       </c>
-      <c r="F4" s="64" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" s="64" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" s="64" t="n">
-        <v>1</v>
-      </c>
-      <c r="I4" s="64" t="n">
-        <v>1</v>
-      </c>
-      <c r="J4" s="64" t="n">
-        <v>1</v>
-      </c>
-      <c r="K4" s="65" t="n">
+      <c r="D4" s="64" t="s">
+        <v>115</v>
+      </c>
+      <c r="E4" s="65" t="s">
+        <v>116</v>
+      </c>
+      <c r="F4" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" s="67" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="66" t="s">
+      <c r="A5" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="62" t="s">
+      <c r="B5" s="64" t="s">
+        <v>117</v>
+      </c>
+      <c r="C5" s="65" t="s">
+        <v>118</v>
+      </c>
+      <c r="D5" s="64" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="69" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="67" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="68" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="64" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6" s="65" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6" s="64" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="69" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" s="67" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="68" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="64" t="s">
+        <v>121</v>
+      </c>
+      <c r="C7" s="65" t="s">
+        <v>122</v>
+      </c>
+      <c r="D7" s="64" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="65" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="67" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="70" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="71" t="s">
+        <v>123</v>
+      </c>
+      <c r="C8" s="72" t="s">
+        <v>124</v>
+      </c>
+      <c r="D8" s="73" t="s">
         <v>115</v>
       </c>
-      <c r="C5" s="63" t="s">
+      <c r="E8" s="74" t="s">
         <v>116</v>
       </c>
-      <c r="D5" s="62" t="s">
-        <v>53</v>
-      </c>
-      <c r="E5" s="67" t="s">
+      <c r="F8" s="75" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="75" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" s="75" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" s="75" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" s="75" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" s="76" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="68" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="64" t="s">
+        <v>125</v>
+      </c>
+      <c r="C9" s="65" t="s">
+        <v>126</v>
+      </c>
+      <c r="D9" s="64" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="65" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="64" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" s="64" t="n">
-        <v>1</v>
-      </c>
-      <c r="H5" s="64" t="n">
-        <v>1</v>
-      </c>
-      <c r="I5" s="64" t="n">
-        <v>1</v>
-      </c>
-      <c r="J5" s="64" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" s="65" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="66" t="s">
+      <c r="F9" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="I9" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" s="67" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="62" t="s">
-        <v>117</v>
-      </c>
-      <c r="C6" s="63" t="s">
-        <v>118</v>
-      </c>
-      <c r="D6" s="62" t="s">
-        <v>53</v>
-      </c>
-      <c r="E6" s="67" t="s">
-        <v>42</v>
-      </c>
-      <c r="F6" s="64" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" s="64" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" s="64" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" s="64" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" s="64" t="n">
-        <v>0</v>
-      </c>
-      <c r="K6" s="65" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="66" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="62" t="s">
-        <v>119</v>
-      </c>
-      <c r="C7" s="63" t="s">
-        <v>120</v>
-      </c>
-      <c r="D7" s="62" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" s="63" t="s">
-        <v>42</v>
-      </c>
-      <c r="F7" s="64" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" s="64" t="n">
-        <v>1</v>
-      </c>
-      <c r="H7" s="64" t="n">
-        <v>1</v>
-      </c>
-      <c r="I7" s="64" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" s="64" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" s="65" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="68" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="69" t="s">
-        <v>121</v>
-      </c>
-      <c r="C8" s="70" t="s">
-        <v>122</v>
-      </c>
-      <c r="D8" s="71" t="s">
-        <v>113</v>
-      </c>
-      <c r="E8" s="72" t="s">
-        <v>114</v>
-      </c>
-      <c r="F8" s="73" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" s="73" t="n">
-        <v>1</v>
-      </c>
-      <c r="H8" s="73" t="n">
-        <v>1</v>
-      </c>
-      <c r="I8" s="73" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" s="73" t="n">
-        <v>0</v>
-      </c>
-      <c r="K8" s="74" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="66" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="62" t="s">
-        <v>123</v>
-      </c>
-      <c r="C9" s="63" t="s">
-        <v>124</v>
-      </c>
-      <c r="D9" s="62" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" s="63" t="s">
-        <v>42</v>
-      </c>
-      <c r="F9" s="64" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" s="64" t="n">
-        <v>1</v>
-      </c>
-      <c r="H9" s="64" t="n">
-        <v>1</v>
-      </c>
-      <c r="I9" s="64" t="n">
-        <v>1</v>
-      </c>
-      <c r="J9" s="64" t="n">
-        <v>0</v>
-      </c>
-      <c r="K9" s="65" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="68" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="69" t="s">
-        <v>125</v>
-      </c>
-      <c r="C10" s="70" t="s">
-        <v>126</v>
-      </c>
-      <c r="D10" s="71" t="s">
-        <v>113</v>
-      </c>
-      <c r="E10" s="72" t="s">
-        <v>114</v>
-      </c>
-      <c r="F10" s="73" t="n">
-        <v>0</v>
-      </c>
-      <c r="G10" s="73" t="n">
-        <v>1</v>
-      </c>
-      <c r="H10" s="73" t="n">
-        <v>1</v>
-      </c>
-      <c r="I10" s="73" t="n">
-        <v>1</v>
-      </c>
-      <c r="J10" s="73" t="n">
-        <v>0</v>
-      </c>
-      <c r="K10" s="74" t="n">
+      <c r="B10" s="71" t="s">
+        <v>127</v>
+      </c>
+      <c r="C10" s="72" t="s">
+        <v>128</v>
+      </c>
+      <c r="D10" s="73" t="s">
+        <v>115</v>
+      </c>
+      <c r="E10" s="74" t="s">
+        <v>116</v>
+      </c>
+      <c r="F10" s="75" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="75" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" s="75" t="n">
+        <v>1</v>
+      </c>
+      <c r="I10" s="75" t="n">
+        <v>1</v>
+      </c>
+      <c r="J10" s="75" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" s="76" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="66"/>
-      <c r="B11" s="75"/>
-      <c r="C11" s="76"/>
-      <c r="D11" s="77"/>
-      <c r="E11" s="78"/>
-      <c r="F11" s="79"/>
-      <c r="G11" s="79"/>
-      <c r="H11" s="79"/>
-      <c r="I11" s="79"/>
+      <c r="A11" s="68"/>
+      <c r="B11" s="77"/>
+      <c r="C11" s="78"/>
+      <c r="D11" s="79"/>
+      <c r="E11" s="80"/>
+      <c r="F11" s="81"/>
+      <c r="G11" s="81"/>
+      <c r="H11" s="81"/>
+      <c r="I11" s="81"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="59"/>
-      <c r="B12" s="75"/>
-      <c r="C12" s="80"/>
-      <c r="D12" s="77"/>
-      <c r="E12" s="78"/>
-      <c r="F12" s="79"/>
-      <c r="G12" s="79"/>
-      <c r="H12" s="79"/>
-      <c r="I12" s="79"/>
+      <c r="A12" s="61"/>
+      <c r="B12" s="77"/>
+      <c r="C12" s="82"/>
+      <c r="D12" s="79"/>
+      <c r="E12" s="80"/>
+      <c r="F12" s="81"/>
+      <c r="G12" s="81"/>
+      <c r="H12" s="81"/>
+      <c r="I12" s="81"/>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="66"/>
-      <c r="B13" s="75"/>
-      <c r="C13" s="81"/>
-      <c r="D13" s="77"/>
-      <c r="E13" s="78"/>
-      <c r="F13" s="79"/>
-      <c r="G13" s="82"/>
-      <c r="H13" s="79"/>
-      <c r="I13" s="79"/>
+      <c r="A13" s="68"/>
+      <c r="B13" s="77"/>
+      <c r="C13" s="83"/>
+      <c r="D13" s="79"/>
+      <c r="E13" s="80"/>
+      <c r="F13" s="81"/>
+      <c r="G13" s="84"/>
+      <c r="H13" s="81"/>
+      <c r="I13" s="81"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="59"/>
-      <c r="B14" s="75"/>
-      <c r="C14" s="81"/>
-      <c r="D14" s="77"/>
-      <c r="E14" s="78"/>
-      <c r="F14" s="79"/>
-      <c r="G14" s="82"/>
-      <c r="H14" s="79"/>
-      <c r="I14" s="79"/>
+      <c r="A14" s="61"/>
+      <c r="B14" s="77"/>
+      <c r="C14" s="83"/>
+      <c r="D14" s="79"/>
+      <c r="E14" s="80"/>
+      <c r="F14" s="81"/>
+      <c r="G14" s="84"/>
+      <c r="H14" s="81"/>
+      <c r="I14" s="81"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3575,26 +3609,26 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
+      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="83" width="31.17004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="83" width="43.0607287449393"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="83" width="18.7449392712551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="83" width="17.5668016194332"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="83" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="83" width="17.8906882591093"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="84" width="8.89068825910931"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="85" width="30.8502024291498"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="85" width="42.6315789473684"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="85" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="85" width="17.4615384615385"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="85" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="85" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="86" width="8.89068825910931"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="85"/>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
+      <c r="A1" s="87"/>
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
       <c r="F1" s="24" t="s">
         <v>27</v>
       </c>
@@ -3606,19 +3640,19 @@
       <c r="L1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="86" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="87" t="s">
+      <c r="A2" s="88" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="89" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="87" t="s">
+      <c r="C2" s="89" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="87" t="s">
+      <c r="D2" s="89" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="87" t="s">
+      <c r="E2" s="89" t="s">
         <v>31</v>
       </c>
       <c r="F2" s="27" t="s">
@@ -3628,13 +3662,13 @@
         <v>33</v>
       </c>
       <c r="H2" s="27" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="I2" s="27" t="s">
         <v>35</v>
       </c>
       <c r="J2" s="27" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="K2" s="27" t="s">
         <v>37</v>
@@ -3644,7 +3678,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="61" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="29" t="s">
@@ -3659,30 +3693,30 @@
       <c r="E3" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="F3" s="88" t="n">
-        <v>2</v>
-      </c>
-      <c r="G3" s="88" t="n">
-        <v>2</v>
-      </c>
-      <c r="H3" s="88" t="n">
-        <v>2</v>
-      </c>
-      <c r="I3" s="88" t="n">
-        <v>2</v>
-      </c>
-      <c r="J3" s="88" t="n">
-        <v>2</v>
-      </c>
-      <c r="K3" s="88" t="n">
-        <v>1</v>
-      </c>
-      <c r="L3" s="89" t="n">
+      <c r="F3" s="90" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3" s="90" t="n">
+        <v>2</v>
+      </c>
+      <c r="H3" s="90" t="n">
+        <v>2</v>
+      </c>
+      <c r="I3" s="90" t="n">
+        <v>2</v>
+      </c>
+      <c r="J3" s="90" t="n">
+        <v>2</v>
+      </c>
+      <c r="K3" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="L3" s="91" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="59" t="s">
+      <c r="A4" s="61" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="29" t="s">
@@ -3697,26 +3731,26 @@
       <c r="E4" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="F4" s="88" t="n">
-        <v>2</v>
-      </c>
-      <c r="G4" s="88" t="n">
-        <v>2</v>
-      </c>
-      <c r="H4" s="88" t="n">
-        <v>2</v>
-      </c>
-      <c r="I4" s="88" t="n">
-        <v>2</v>
-      </c>
-      <c r="J4" s="88" t="n">
-        <v>2</v>
-      </c>
-      <c r="K4" s="88"/>
-      <c r="L4" s="89"/>
+      <c r="F4" s="90" t="n">
+        <v>2</v>
+      </c>
+      <c r="G4" s="90" t="n">
+        <v>2</v>
+      </c>
+      <c r="H4" s="90" t="n">
+        <v>2</v>
+      </c>
+      <c r="I4" s="90" t="n">
+        <v>2</v>
+      </c>
+      <c r="J4" s="90" t="n">
+        <v>2</v>
+      </c>
+      <c r="K4" s="90"/>
+      <c r="L4" s="91"/>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="59" t="s">
+      <c r="A5" s="61" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="29" t="s">
@@ -3731,30 +3765,30 @@
       <c r="E5" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="88" t="n">
-        <v>2</v>
-      </c>
-      <c r="G5" s="88" t="n">
-        <v>2</v>
-      </c>
-      <c r="H5" s="88" t="n">
-        <v>2</v>
-      </c>
-      <c r="I5" s="88" t="n">
-        <v>2</v>
-      </c>
-      <c r="J5" s="88" t="n">
-        <v>2</v>
-      </c>
-      <c r="K5" s="88" t="n">
-        <v>1</v>
-      </c>
-      <c r="L5" s="89" t="n">
+      <c r="F5" s="90" t="n">
+        <v>2</v>
+      </c>
+      <c r="G5" s="90" t="n">
+        <v>2</v>
+      </c>
+      <c r="H5" s="90" t="n">
+        <v>2</v>
+      </c>
+      <c r="I5" s="90" t="n">
+        <v>2</v>
+      </c>
+      <c r="J5" s="90" t="n">
+        <v>2</v>
+      </c>
+      <c r="K5" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="L5" s="91" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="59" t="s">
+      <c r="A6" s="61" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="29" t="s">
@@ -3769,26 +3803,26 @@
       <c r="E6" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="F6" s="88" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" s="88" t="n">
-        <v>1</v>
-      </c>
-      <c r="H6" s="88"/>
-      <c r="I6" s="88" t="n">
-        <v>2</v>
-      </c>
-      <c r="J6" s="88"/>
-      <c r="K6" s="88" t="n">
-        <v>1</v>
-      </c>
-      <c r="L6" s="89" t="n">
+      <c r="F6" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" s="90"/>
+      <c r="I6" s="90" t="n">
+        <v>2</v>
+      </c>
+      <c r="J6" s="90"/>
+      <c r="K6" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="L6" s="91" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="59" t="s">
+      <c r="A7" s="61" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="29" t="s">
@@ -3803,22 +3837,22 @@
       <c r="E7" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="88" t="n">
-        <v>1</v>
-      </c>
-      <c r="G7" s="88" t="n">
-        <v>1</v>
-      </c>
-      <c r="H7" s="88" t="n">
-        <v>2</v>
-      </c>
-      <c r="I7" s="88"/>
-      <c r="J7" s="88"/>
-      <c r="K7" s="88"/>
-      <c r="L7" s="89"/>
+      <c r="F7" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" s="90" t="n">
+        <v>2</v>
+      </c>
+      <c r="I7" s="90"/>
+      <c r="J7" s="90"/>
+      <c r="K7" s="90"/>
+      <c r="L7" s="91"/>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="59" t="s">
+      <c r="A8" s="61" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="29" t="s">
@@ -3833,28 +3867,28 @@
       <c r="E8" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="F8" s="90" t="n">
+      <c r="F8" s="92" t="n">
         <v>3</v>
       </c>
-      <c r="G8" s="88" t="n">
+      <c r="G8" s="90" t="n">
         <v>3</v>
       </c>
-      <c r="H8" s="88" t="n">
+      <c r="H8" s="90" t="n">
         <v>3</v>
       </c>
-      <c r="I8" s="88" t="n">
-        <v>2</v>
-      </c>
-      <c r="J8" s="88" t="n">
-        <v>2</v>
-      </c>
-      <c r="K8" s="88"/>
-      <c r="L8" s="89" t="n">
+      <c r="I8" s="90" t="n">
+        <v>2</v>
+      </c>
+      <c r="J8" s="90" t="n">
+        <v>2</v>
+      </c>
+      <c r="K8" s="90"/>
+      <c r="L8" s="91" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="59" t="s">
+      <c r="A9" s="61" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="29" t="s">
@@ -3869,26 +3903,26 @@
       <c r="E9" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="F9" s="90" t="n">
-        <v>2</v>
-      </c>
-      <c r="G9" s="88" t="n">
-        <v>2</v>
-      </c>
-      <c r="H9" s="88" t="n">
-        <v>2</v>
-      </c>
-      <c r="I9" s="88" t="n">
-        <v>2</v>
-      </c>
-      <c r="J9" s="88"/>
-      <c r="K9" s="88"/>
-      <c r="L9" s="89" t="n">
+      <c r="F9" s="92" t="n">
+        <v>2</v>
+      </c>
+      <c r="G9" s="90" t="n">
+        <v>2</v>
+      </c>
+      <c r="H9" s="90" t="n">
+        <v>2</v>
+      </c>
+      <c r="I9" s="90" t="n">
+        <v>2</v>
+      </c>
+      <c r="J9" s="90"/>
+      <c r="K9" s="90"/>
+      <c r="L9" s="91" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="59" t="s">
+      <c r="A10" s="61" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="29" t="s">
@@ -3903,28 +3937,28 @@
       <c r="E10" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="90" t="n">
-        <v>2</v>
-      </c>
-      <c r="G10" s="88" t="n">
-        <v>2</v>
-      </c>
-      <c r="H10" s="88" t="n">
-        <v>2</v>
-      </c>
-      <c r="I10" s="88" t="n">
-        <v>2</v>
-      </c>
-      <c r="J10" s="88" t="n">
-        <v>2</v>
-      </c>
-      <c r="K10" s="88" t="n">
-        <v>2</v>
-      </c>
-      <c r="L10" s="89"/>
+      <c r="F10" s="92" t="n">
+        <v>2</v>
+      </c>
+      <c r="G10" s="90" t="n">
+        <v>2</v>
+      </c>
+      <c r="H10" s="90" t="n">
+        <v>2</v>
+      </c>
+      <c r="I10" s="90" t="n">
+        <v>2</v>
+      </c>
+      <c r="J10" s="90" t="n">
+        <v>2</v>
+      </c>
+      <c r="K10" s="90" t="n">
+        <v>2</v>
+      </c>
+      <c r="L10" s="91"/>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="59" t="s">
+      <c r="A11" s="61" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="29" t="s">
@@ -3939,28 +3973,28 @@
       <c r="E11" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="F11" s="90" t="n">
-        <v>2</v>
-      </c>
-      <c r="G11" s="90" t="n">
+      <c r="F11" s="92" t="n">
+        <v>2</v>
+      </c>
+      <c r="G11" s="92" t="n">
         <v>3</v>
       </c>
-      <c r="H11" s="90" t="n">
-        <v>2</v>
-      </c>
-      <c r="I11" s="88" t="n">
-        <v>1</v>
-      </c>
-      <c r="J11" s="88" t="n">
-        <v>1</v>
-      </c>
-      <c r="K11" s="88" t="n">
-        <v>2</v>
-      </c>
-      <c r="L11" s="89"/>
+      <c r="H11" s="92" t="n">
+        <v>2</v>
+      </c>
+      <c r="I11" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="J11" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="K11" s="90" t="n">
+        <v>2</v>
+      </c>
+      <c r="L11" s="91"/>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="59" t="s">
+      <c r="A12" s="61" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="29" t="s">
@@ -3975,26 +4009,26 @@
       <c r="E12" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="F12" s="90" t="n">
-        <v>2</v>
-      </c>
-      <c r="G12" s="90" t="n">
+      <c r="F12" s="92" t="n">
+        <v>2</v>
+      </c>
+      <c r="G12" s="92" t="n">
         <v>3</v>
       </c>
-      <c r="H12" s="90" t="n">
-        <v>2</v>
-      </c>
-      <c r="I12" s="88" t="n">
-        <v>1</v>
-      </c>
-      <c r="J12" s="88" t="n">
-        <v>1</v>
-      </c>
-      <c r="K12" s="88"/>
-      <c r="L12" s="89"/>
+      <c r="H12" s="92" t="n">
+        <v>2</v>
+      </c>
+      <c r="I12" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="J12" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="K12" s="90"/>
+      <c r="L12" s="91"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="59" t="s">
+      <c r="A13" s="61" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="29" t="s">
@@ -4009,24 +4043,24 @@
       <c r="E13" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="F13" s="90" t="n">
-        <v>1</v>
-      </c>
-      <c r="G13" s="90" t="n">
-        <v>2</v>
-      </c>
-      <c r="H13" s="90" t="n">
-        <v>1</v>
-      </c>
-      <c r="I13" s="88" t="n">
-        <v>1</v>
-      </c>
-      <c r="J13" s="88"/>
-      <c r="K13" s="88"/>
-      <c r="L13" s="89"/>
+      <c r="F13" s="92" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" s="92" t="n">
+        <v>2</v>
+      </c>
+      <c r="H13" s="92" t="n">
+        <v>1</v>
+      </c>
+      <c r="I13" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="J13" s="90"/>
+      <c r="K13" s="90"/>
+      <c r="L13" s="91"/>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="59" t="s">
+      <c r="A14" s="61" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="29" t="s">
@@ -4041,26 +4075,26 @@
       <c r="E14" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="F14" s="90" t="n">
-        <v>2</v>
-      </c>
-      <c r="G14" s="90" t="n">
-        <v>2</v>
-      </c>
-      <c r="H14" s="90" t="n">
-        <v>2</v>
-      </c>
-      <c r="I14" s="88" t="n">
-        <v>1</v>
-      </c>
-      <c r="J14" s="88" t="n">
-        <v>1</v>
-      </c>
-      <c r="K14" s="88"/>
-      <c r="L14" s="89"/>
+      <c r="F14" s="92" t="n">
+        <v>2</v>
+      </c>
+      <c r="G14" s="92" t="n">
+        <v>2</v>
+      </c>
+      <c r="H14" s="92" t="n">
+        <v>2</v>
+      </c>
+      <c r="I14" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="J14" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="K14" s="90"/>
+      <c r="L14" s="91"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="59" t="s">
+      <c r="A15" s="61" t="s">
         <v>12</v>
       </c>
       <c r="B15" s="29" t="s">
@@ -4075,24 +4109,24 @@
       <c r="E15" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="F15" s="90" t="n">
-        <v>2</v>
-      </c>
-      <c r="G15" s="90" t="n">
-        <v>2</v>
-      </c>
-      <c r="H15" s="90" t="n">
-        <v>2</v>
-      </c>
-      <c r="I15" s="88" t="n">
-        <v>1</v>
-      </c>
-      <c r="J15" s="88"/>
-      <c r="K15" s="88"/>
-      <c r="L15" s="89"/>
+      <c r="F15" s="92" t="n">
+        <v>2</v>
+      </c>
+      <c r="G15" s="92" t="n">
+        <v>2</v>
+      </c>
+      <c r="H15" s="92" t="n">
+        <v>2</v>
+      </c>
+      <c r="I15" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="J15" s="90"/>
+      <c r="K15" s="90"/>
+      <c r="L15" s="91"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="59" t="s">
+      <c r="A16" s="61" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="29" t="s">
@@ -4107,30 +4141,30 @@
       <c r="E16" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="F16" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="G16" s="88" t="n">
-        <v>2</v>
-      </c>
-      <c r="H16" s="88" t="n">
-        <v>2</v>
-      </c>
-      <c r="I16" s="88" t="n">
-        <v>2</v>
-      </c>
-      <c r="J16" s="88" t="n">
-        <v>1</v>
-      </c>
-      <c r="K16" s="88" t="n">
-        <v>1</v>
-      </c>
-      <c r="L16" s="89" t="n">
+      <c r="F16" s="92" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" s="90" t="n">
+        <v>2</v>
+      </c>
+      <c r="H16" s="90" t="n">
+        <v>2</v>
+      </c>
+      <c r="I16" s="90" t="n">
+        <v>2</v>
+      </c>
+      <c r="J16" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="K16" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="L16" s="91" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="59" t="s">
+      <c r="A17" s="61" t="s">
         <v>12</v>
       </c>
       <c r="B17" s="29" t="s">
@@ -4145,30 +4179,30 @@
       <c r="E17" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="F17" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="G17" s="88" t="n">
-        <v>2</v>
-      </c>
-      <c r="H17" s="88" t="n">
-        <v>2</v>
-      </c>
-      <c r="I17" s="88" t="n">
-        <v>2</v>
-      </c>
-      <c r="J17" s="88" t="n">
-        <v>1</v>
-      </c>
-      <c r="K17" s="88" t="n">
-        <v>1</v>
-      </c>
-      <c r="L17" s="89" t="n">
+      <c r="F17" s="92" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" s="90" t="n">
+        <v>2</v>
+      </c>
+      <c r="H17" s="90" t="n">
+        <v>2</v>
+      </c>
+      <c r="I17" s="90" t="n">
+        <v>2</v>
+      </c>
+      <c r="J17" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="K17" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="L17" s="91" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="59" t="s">
+      <c r="A18" s="61" t="s">
         <v>12</v>
       </c>
       <c r="B18" s="29" t="s">
@@ -4183,30 +4217,30 @@
       <c r="E18" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="F18" s="90" t="n">
-        <v>2</v>
-      </c>
-      <c r="G18" s="88" t="n">
+      <c r="F18" s="92" t="n">
+        <v>2</v>
+      </c>
+      <c r="G18" s="90" t="n">
         <v>4</v>
       </c>
-      <c r="H18" s="88" t="n">
-        <v>2</v>
-      </c>
-      <c r="I18" s="88" t="n">
-        <v>2</v>
-      </c>
-      <c r="J18" s="88" t="n">
-        <v>1</v>
-      </c>
-      <c r="K18" s="88" t="n">
-        <v>1</v>
-      </c>
-      <c r="L18" s="89" t="n">
+      <c r="H18" s="90" t="n">
+        <v>2</v>
+      </c>
+      <c r="I18" s="90" t="n">
+        <v>2</v>
+      </c>
+      <c r="J18" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="K18" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="L18" s="91" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="59" t="s">
+      <c r="A19" s="61" t="s">
         <v>12</v>
       </c>
       <c r="B19" s="29" t="s">
@@ -4221,28 +4255,28 @@
       <c r="E19" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="F19" s="90" t="n">
-        <v>2</v>
-      </c>
-      <c r="G19" s="88" t="n">
+      <c r="F19" s="92" t="n">
+        <v>2</v>
+      </c>
+      <c r="G19" s="90" t="n">
         <v>4</v>
       </c>
-      <c r="H19" s="88" t="n">
-        <v>2</v>
-      </c>
-      <c r="I19" s="88" t="n">
-        <v>1</v>
-      </c>
-      <c r="J19" s="88" t="n">
-        <v>1</v>
-      </c>
-      <c r="K19" s="88"/>
-      <c r="L19" s="89" t="n">
+      <c r="H19" s="90" t="n">
+        <v>2</v>
+      </c>
+      <c r="I19" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="J19" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="K19" s="90"/>
+      <c r="L19" s="91" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="91" t="s">
+      <c r="A20" s="93" t="s">
         <v>12</v>
       </c>
       <c r="B20" s="29" t="s">
@@ -4257,30 +4291,30 @@
       <c r="E20" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="F20" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="G20" s="88" t="n">
-        <v>1</v>
-      </c>
-      <c r="H20" s="88" t="n">
-        <v>1</v>
-      </c>
-      <c r="I20" s="88" t="n">
-        <v>1</v>
-      </c>
-      <c r="J20" s="88" t="n">
-        <v>1</v>
-      </c>
-      <c r="K20" s="88" t="n">
-        <v>1</v>
-      </c>
-      <c r="L20" s="88" t="n">
+      <c r="F20" s="92" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="H20" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="I20" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="J20" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="K20" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="L20" s="90" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="91" t="s">
+      <c r="A21" s="93" t="s">
         <v>12</v>
       </c>
       <c r="B21" s="29" t="s">
@@ -4295,175 +4329,175 @@
       <c r="E21" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="F21" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="G21" s="88" t="n">
-        <v>1</v>
-      </c>
-      <c r="H21" s="88" t="n">
-        <v>1</v>
-      </c>
-      <c r="I21" s="88" t="n">
-        <v>1</v>
-      </c>
-      <c r="J21" s="88" t="n">
-        <v>1</v>
-      </c>
-      <c r="K21" s="88"/>
-      <c r="L21" s="88" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="92" t="s">
-        <v>128</v>
-      </c>
-      <c r="B22" s="62" t="s">
+      <c r="F21" s="92" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="H21" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="I21" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="J21" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="K21" s="90"/>
+      <c r="L21" s="90" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="94" t="s">
+        <v>130</v>
+      </c>
+      <c r="B22" s="64" t="s">
+        <v>117</v>
+      </c>
+      <c r="C22" s="65" t="s">
+        <v>118</v>
+      </c>
+      <c r="D22" s="64" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22" s="69" t="s">
+        <v>42</v>
+      </c>
+      <c r="F22" s="92" t="n">
+        <v>3</v>
+      </c>
+      <c r="G22" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" s="90" t="n">
+        <v>3</v>
+      </c>
+      <c r="I22" s="90" t="n">
+        <v>3</v>
+      </c>
+      <c r="J22" s="90" t="n">
+        <v>3</v>
+      </c>
+      <c r="K22" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="L22" s="90" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="94" t="s">
+        <v>130</v>
+      </c>
+      <c r="B23" s="64" t="s">
+        <v>119</v>
+      </c>
+      <c r="C23" s="65" t="s">
+        <v>120</v>
+      </c>
+      <c r="D23" s="64" t="s">
+        <v>53</v>
+      </c>
+      <c r="E23" s="69" t="s">
+        <v>42</v>
+      </c>
+      <c r="F23" s="92" t="n">
+        <v>10</v>
+      </c>
+      <c r="G23" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="I23" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="K23" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="L23" s="90" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="94" t="s">
+        <v>130</v>
+      </c>
+      <c r="B24" s="64" t="s">
+        <v>125</v>
+      </c>
+      <c r="C24" s="65" t="s">
+        <v>126</v>
+      </c>
+      <c r="D24" s="64" t="s">
+        <v>41</v>
+      </c>
+      <c r="E24" s="65" t="s">
+        <v>42</v>
+      </c>
+      <c r="F24" s="92" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="H24" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="I24" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="J24" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="K24" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="L24" s="90" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="94" t="s">
+        <v>130</v>
+      </c>
+      <c r="B25" s="62" t="s">
+        <v>127</v>
+      </c>
+      <c r="C25" s="65" t="s">
+        <v>131</v>
+      </c>
+      <c r="D25" s="95" t="s">
         <v>115</v>
       </c>
-      <c r="C22" s="63" t="s">
+      <c r="E25" s="96" t="s">
         <v>116</v>
       </c>
-      <c r="D22" s="62" t="s">
-        <v>53</v>
-      </c>
-      <c r="E22" s="67" t="s">
-        <v>42</v>
-      </c>
-      <c r="F22" s="90" t="n">
-        <v>3</v>
-      </c>
-      <c r="G22" s="88" t="n">
-        <v>0</v>
-      </c>
-      <c r="H22" s="88" t="n">
-        <v>3</v>
-      </c>
-      <c r="I22" s="88" t="n">
-        <v>3</v>
-      </c>
-      <c r="J22" s="88" t="n">
-        <v>3</v>
-      </c>
-      <c r="K22" s="88" t="n">
-        <v>0</v>
-      </c>
-      <c r="L22" s="88" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="92" t="s">
-        <v>128</v>
-      </c>
-      <c r="B23" s="62" t="s">
-        <v>117</v>
-      </c>
-      <c r="C23" s="63" t="s">
-        <v>118</v>
-      </c>
-      <c r="D23" s="62" t="s">
-        <v>53</v>
-      </c>
-      <c r="E23" s="67" t="s">
-        <v>42</v>
-      </c>
-      <c r="F23" s="90" t="n">
-        <v>10</v>
-      </c>
-      <c r="G23" s="88" t="n">
-        <v>0</v>
-      </c>
-      <c r="H23" s="88" t="n">
-        <v>0</v>
-      </c>
-      <c r="I23" s="88" t="n">
-        <v>0</v>
-      </c>
-      <c r="J23" s="88" t="n">
-        <v>0</v>
-      </c>
-      <c r="K23" s="88" t="n">
-        <v>0</v>
-      </c>
-      <c r="L23" s="88" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="92" t="s">
-        <v>128</v>
-      </c>
-      <c r="B24" s="62" t="s">
-        <v>123</v>
-      </c>
-      <c r="C24" s="63" t="s">
-        <v>124</v>
-      </c>
-      <c r="D24" s="62" t="s">
-        <v>41</v>
-      </c>
-      <c r="E24" s="63" t="s">
-        <v>42</v>
-      </c>
-      <c r="F24" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="G24" s="88" t="n">
-        <v>1</v>
-      </c>
-      <c r="H24" s="88" t="n">
-        <v>1</v>
-      </c>
-      <c r="I24" s="88" t="n">
-        <v>1</v>
-      </c>
-      <c r="J24" s="88" t="n">
-        <v>1</v>
-      </c>
-      <c r="K24" s="88" t="n">
-        <v>1</v>
-      </c>
-      <c r="L24" s="88" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="92" t="s">
-        <v>128</v>
-      </c>
-      <c r="B25" s="60" t="s">
-        <v>125</v>
-      </c>
-      <c r="C25" s="63" t="s">
-        <v>129</v>
-      </c>
-      <c r="D25" s="62" t="s">
-        <v>113</v>
-      </c>
-      <c r="E25" s="67" t="s">
-        <v>114</v>
-      </c>
-      <c r="F25" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="G25" s="88" t="n">
-        <v>0</v>
-      </c>
-      <c r="H25" s="88" t="n">
-        <v>1</v>
-      </c>
-      <c r="I25" s="88" t="n">
-        <v>1</v>
-      </c>
-      <c r="J25" s="88" t="n">
-        <v>1</v>
-      </c>
-      <c r="K25" s="88" t="n">
-        <v>1</v>
-      </c>
-      <c r="L25" s="88" t="n">
+      <c r="F25" s="92" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="I25" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="J25" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="K25" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="L25" s="90" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4472,7 +4506,7 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A3:A22" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A3:A21" type="list">
       <formula1>"Product Minimum Facings Primary,Product Minimum Facing Secondary "</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
SanofiZA - template fix
</commit_message>
<xml_diff>
--- a/Projects/SANOFIZA/Data/Template.xlsx
+++ b/Projects/SANOFIZA/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,6 +15,10 @@
     <sheet name="Primary&amp;Secondary_POSM" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="Primary&amp;Secondary_Facings" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">MSL!$A$2:$L$23</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">MSL!$A$2:$L$23</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -447,7 +451,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="118">
   <si>
     <t xml:space="preserve">KPI Name</t>
   </si>
@@ -689,115 +693,118 @@
     <t xml:space="preserve">6006127000347</t>
   </si>
   <si>
+    <t xml:space="preserve">Buscopan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buscopan syrup 100ml </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6006127000408</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antistax tabs 30s </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6006127001580</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antistax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Preventative Care</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antistax tabs 60s </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6006127001498</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Telfast Susp.150ml </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6009609472335</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Telfast </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allergy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Telfast tabs 120mg 30s </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6005317003151</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKUs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mega</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Community Low </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SA Dulcolax Shelf trays </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SA _DUL_ST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SA Antistax Shelf tray</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SA-ANT-ST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S Essentiale Shelf Talker/Strip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S-STS-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SA Counter Unit </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SA-CTU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multibrand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multicategory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SA Clip Strip </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SA CS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SA  FSU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S-FSU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S Dis-Chem Q1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S-POSM-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mega Pharmacies</t>
+  </si>
+  <si>
     <t xml:space="preserve">Buscopan </t>
   </si>
   <si>
-    <t xml:space="preserve">Pain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Buscopan syrup 100ml </t>
-  </si>
-  <si>
-    <t xml:space="preserve">6006127000408</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Antistax tabs 30s </t>
-  </si>
-  <si>
-    <t xml:space="preserve">6006127001580</t>
-  </si>
-  <si>
     <t xml:space="preserve">Antistax </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Preventative Care</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Antistax tabs 60s </t>
-  </si>
-  <si>
-    <t xml:space="preserve">6006127001498</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Telfast Susp.150ml </t>
-  </si>
-  <si>
-    <t xml:space="preserve">6009609472335</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Telfast </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allergy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Telfast tabs 120mg 30s </t>
-  </si>
-  <si>
-    <t xml:space="preserve">6005317003151</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKUs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mega</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Community Low </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SA Dulcolax Shelf trays </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SA _DUL_ST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SA Antistax Shelf tray</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SA-ANT-ST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Antistax</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S Essentiale Shelf Talker/Strip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S-STS-03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SA Counter Unit </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SA-CTU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multibrand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multicategory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SA Clip Strip </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SA CS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SA  FSU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S-FSU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S Dis-Chem Q1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S-POSM-01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mega Pharmacies</t>
   </si>
 </sst>
 </file>
@@ -1610,6 +1617,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -1617,20 +1628,20 @@
   </sheetPr>
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.0647773279352"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.2793522267206"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.8542510121457"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.2105263157895"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.7449392712551"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.0283400809717"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.1417004048583"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1882,25 +1893,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+  <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="25.0647773279352"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="43.0607287449393"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="22.0647773279352"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="17.8906882591093"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="13" width="15.8542510121457"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="17.8906882591093"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="13" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="14" width="8.89068825910931"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="25.9230769230769"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="44.7773279352227"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="13" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="13" width="17.0323886639676"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="14" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2337,7 +2348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="20" t="s">
         <v>23</v>
       </c>
@@ -2375,7 +2386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="14.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="20" t="s">
         <v>23</v>
       </c>
@@ -2413,7 +2424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="14.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="20" t="s">
         <v>23</v>
       </c>
@@ -2527,7 +2538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="20" t="s">
         <v>23</v>
       </c>
@@ -2565,7 +2576,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0"/>
       <c r="B19" s="21" t="s">
         <v>82</v>
       </c>
@@ -2601,6 +2613,9 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="20" t="s">
+        <v>23</v>
+      </c>
       <c r="B20" s="21" t="s">
         <v>84</v>
       </c>
@@ -2636,6 +2651,9 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="20" t="s">
+        <v>23</v>
+      </c>
       <c r="B21" s="21" t="s">
         <v>88</v>
       </c>
@@ -2670,7 +2688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="21" t="s">
         <v>90</v>
       </c>
@@ -2705,7 +2723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="21" t="s">
         <v>94</v>
       </c>
@@ -2740,7 +2758,15 @@
         <v>1</v>
       </c>
     </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <autoFilter ref="A2:L23">
+    <filterColumn colId="5">
+      <customFilters and="true">
+        <customFilter operator="equal" val="1"/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="F1:G1"/>
   </mergeCells>
@@ -2751,7 +2777,8 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <legacyDrawing r:id="rId2"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -2762,18 +2789,18 @@
   </sheetPr>
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B35" activeCellId="0" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="25.8137651821862"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="29" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="29" width="32.1376518218623"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="29" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="29" width="17.8906882591093"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="14" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="26.8866396761134"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="29" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="29" width="33.4210526315789"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="29" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="29" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="14" width="9.31983805668016"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3002,18 +3029,18 @@
   </sheetPr>
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="35" width="20.7813765182186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="35" width="66.412955465587"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="35" width="41.668016194332"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="35" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="35" width="14.8906882591093"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="36" width="8.89068825910931"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="35" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="35" width="68.9838056680162"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="35" width="43.3846153846154"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="35" width="17.0323886639676"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="35" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="36" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3442,24 +3469,24 @@
   </sheetPr>
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="28.4939271255061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="49" width="32.3481781376518"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="29" width="22.0647773279352"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="49" width="26.3522267206478"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="49" width="21.1012145748988"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="29" width="18.5303643724696"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="29" width="17.8906882591093"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="50" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="50" width="10.1781376518219"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="50" width="8.89068825910931"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="50" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="50" width="8.89068825910931"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="29.5668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="49" width="33.8502024291498"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="29" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="49" width="27.3157894736842"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="49" width="21.9595141700405"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="29" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="29" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="50" width="10.6032388663968"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="50" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="50" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="50" width="11.0323886639676"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="50" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3565,7 +3592,7 @@
         <v>102</v>
       </c>
       <c r="D4" s="56" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="E4" s="57" t="s">
         <v>45</v>
@@ -3597,10 +3624,10 @@
         <v>7</v>
       </c>
       <c r="B5" s="59" t="s">
+        <v>103</v>
+      </c>
+      <c r="C5" s="60" t="s">
         <v>104</v>
-      </c>
-      <c r="C5" s="60" t="s">
-        <v>105</v>
       </c>
       <c r="D5" s="56" t="s">
         <v>56</v>
@@ -3635,16 +3662,16 @@
         <v>20</v>
       </c>
       <c r="B6" s="54" t="s">
+        <v>105</v>
+      </c>
+      <c r="C6" s="64" t="s">
         <v>106</v>
       </c>
-      <c r="C6" s="64" t="s">
+      <c r="D6" s="65" t="s">
         <v>107</v>
       </c>
-      <c r="D6" s="65" t="s">
+      <c r="E6" s="66" t="s">
         <v>108</v>
-      </c>
-      <c r="E6" s="66" t="s">
-        <v>109</v>
       </c>
       <c r="F6" s="34" t="n">
         <v>0</v>
@@ -3673,16 +3700,16 @@
         <v>20</v>
       </c>
       <c r="B7" s="67" t="s">
+        <v>109</v>
+      </c>
+      <c r="C7" s="58" t="s">
         <v>110</v>
       </c>
-      <c r="C7" s="58" t="s">
-        <v>111</v>
-      </c>
       <c r="D7" s="65" t="s">
+        <v>107</v>
+      </c>
+      <c r="E7" s="66" t="s">
         <v>108</v>
-      </c>
-      <c r="E7" s="66" t="s">
-        <v>109</v>
       </c>
       <c r="F7" s="34" t="n">
         <v>0</v>
@@ -3711,16 +3738,16 @@
         <v>20</v>
       </c>
       <c r="B8" s="54" t="s">
+        <v>111</v>
+      </c>
+      <c r="C8" s="64" t="s">
         <v>112</v>
       </c>
-      <c r="C8" s="64" t="s">
-        <v>113</v>
-      </c>
       <c r="D8" s="65" t="s">
+        <v>107</v>
+      </c>
+      <c r="E8" s="66" t="s">
         <v>108</v>
-      </c>
-      <c r="E8" s="66" t="s">
-        <v>109</v>
       </c>
       <c r="F8" s="34" t="n">
         <v>0</v>
@@ -3749,16 +3776,16 @@
         <v>20</v>
       </c>
       <c r="B9" s="69" t="s">
+        <v>113</v>
+      </c>
+      <c r="C9" s="70" t="s">
         <v>114</v>
       </c>
-      <c r="C9" s="70" t="s">
-        <v>115</v>
-      </c>
       <c r="D9" s="70" t="s">
+        <v>107</v>
+      </c>
+      <c r="E9" s="71" t="s">
         <v>108</v>
-      </c>
-      <c r="E9" s="71" t="s">
-        <v>109</v>
       </c>
       <c r="F9" s="72" t="n">
         <v>1</v>
@@ -3807,19 +3834,19 @@
   </sheetPr>
   <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="75" width="31.17004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="75" width="43.0607287449393"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="75" width="18.7449392712551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="75" width="17.5668016194332"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="75" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="8" min="6" style="75" width="17.8906882591093"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="76" width="8.89068825910931"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="75" width="32.2429149797571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="75" width="44.7773279352227"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="75" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="75" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="75" width="17.0323886639676"/>
+    <col collapsed="false" hidden="false" max="8" min="6" style="75" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="76" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3861,7 +3888,7 @@
         <v>36</v>
       </c>
       <c r="H2" s="18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I2" s="18" t="s">
         <v>38</v>
@@ -4457,7 +4484,7 @@
         <v>79</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>80</v>
+        <v>116</v>
       </c>
       <c r="E18" s="21" t="s">
         <v>81</v>
@@ -4495,7 +4522,7 @@
         <v>83</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>80</v>
+        <v>116</v>
       </c>
       <c r="E19" s="21" t="s">
         <v>81</v>
@@ -4533,7 +4560,7 @@
         <v>85</v>
       </c>
       <c r="D20" s="21" t="s">
-        <v>86</v>
+        <v>117</v>
       </c>
       <c r="E20" s="21" t="s">
         <v>87</v>
@@ -4571,7 +4598,7 @@
         <v>89</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>86</v>
+        <v>117</v>
       </c>
       <c r="E21" s="21" t="s">
         <v>87</v>
@@ -4679,16 +4706,16 @@
         <v>20</v>
       </c>
       <c r="B24" s="69" t="s">
+        <v>113</v>
+      </c>
+      <c r="C24" s="70" t="s">
         <v>114</v>
       </c>
-      <c r="C24" s="70" t="s">
-        <v>115</v>
-      </c>
       <c r="D24" s="70" t="s">
+        <v>107</v>
+      </c>
+      <c r="E24" s="71" t="s">
         <v>108</v>
-      </c>
-      <c r="E24" s="71" t="s">
-        <v>109</v>
       </c>
       <c r="F24" s="72" t="n">
         <v>1</v>

</xml_diff>